<commit_message>
Adding new middleman server project and updating other clients with new ipaddresses for middleman
</commit_message>
<xml_diff>
--- a/Documentation/Project2TasksSpreadsheet.xlsx
+++ b/Documentation/Project2TasksSpreadsheet.xlsx
@@ -22,6 +22,103 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="74">
   <si>
+    <t>Jacob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jerrell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Presentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sei Jung</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Requirement number</t>
+  </si>
+  <si>
+    <t>(New Requirements)</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Estimated Time (hours)</t>
+  </si>
+  <si>
+    <t>Risk Value</t>
+  </si>
+  <si>
+    <t>Task Value</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Design new UI on paper to accommodate all new requirements in addition to existing movement GUI</t>
+  </si>
+  <si>
+    <t>Port existing movement GUI to new structure</t>
+  </si>
+  <si>
+    <t>Learn format for GPS coordinates on Android to be used by GUI</t>
+  </si>
+  <si>
+    <t>Android Tablet GUI</t>
+  </si>
+  <si>
+    <t>Create GPS (Waypoint entery and come home) part of GUI</t>
+  </si>
+  <si>
+    <t>Communication between Vex, Phone, and Tablet</t>
+  </si>
+  <si>
+    <t>Create basic UI structure and intgrate with existing client from Android-Android communication</t>
+  </si>
+  <si>
+    <t>Read information on using an Android device as both a send and receive server</t>
+  </si>
+  <si>
+    <t>Code send/receive server on single Android device</t>
+  </si>
+  <si>
+    <t>Test send/receive server as receiver from second Android device</t>
+  </si>
+  <si>
+    <t>Code printing and forwarding of movement commands, and printing of GPS commands, printing of errors for non-recognized commands</t>
+  </si>
+  <si>
+    <t>Test forwarding of movement commands from Tablet to the Vex</t>
+  </si>
+  <si>
+    <t>Android able to get GPS coordinates</t>
+  </si>
+  <si>
+    <t>Read documentation on Android location API and location services API from Google Play SDK</t>
+  </si>
+  <si>
+    <t>Create collection of 5 known GPS locations on campus using Google Maps</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Code basic app that gets the current GPS location when a button is pressed, displaying it to the screen and the time from when the button was pressed to when the GPS location is acquired</t>
+  </si>
+  <si>
+    <t>Add functionality to GPS app that gets current facing direction</t>
+  </si>
+  <si>
+    <t>Test facing direction functionality</t>
+  </si>
+  <si>
+    <t>Test basic GPS locator app at known locations, comparing the results</t>
+  </si>
+  <si>
     <t>Integrate GPS code with existing Phone send/receive server</t>
   </si>
   <si>
@@ -156,110 +253,17 @@
   <si>
     <t>Report</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jacob</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jerrell</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Presentation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sei Jung</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Requirement number</t>
-  </si>
-  <si>
-    <t>(New Requirements)</t>
-  </si>
-  <si>
-    <t>Points</t>
-  </si>
-  <si>
-    <t>Estimated Time (hours)</t>
-  </si>
-  <si>
-    <t>Risk Value</t>
-  </si>
-  <si>
-    <t>Task Value</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Design new UI on paper to accommodate all new requirements in addition to existing movement GUI</t>
-  </si>
-  <si>
-    <t>Port existing movement GUI to new structure</t>
-  </si>
-  <si>
-    <t>Learn format for GPS coordinates on Android to be used by GUI</t>
-  </si>
-  <si>
-    <t>Android Tablet GUI</t>
-  </si>
-  <si>
-    <t>Create GPS (Waypoint entery and come home) part of GUI</t>
-  </si>
-  <si>
-    <t>Communication between Vex, Phone, and Tablet</t>
-  </si>
-  <si>
-    <t>Create basic UI structure and intgrate with existing client from Android-Android communication</t>
-  </si>
-  <si>
-    <t>Read information on using an Android device as both a send and receive server</t>
-  </si>
-  <si>
-    <t>Code send/receive server on single Android device</t>
-  </si>
-  <si>
-    <t>Test send/receive server as receiver from second Android device</t>
-  </si>
-  <si>
-    <t>Code printing and forwarding of movement commands, and printing of GPS commands, printing of errors for non-recognized commands</t>
-  </si>
-  <si>
-    <t>Test forwarding of movement commands from Tablet to the Vex</t>
-  </si>
-  <si>
-    <t>Android able to get GPS coordinates</t>
-  </si>
-  <si>
-    <t>Read documentation on Android location API and location services API from Google Play SDK</t>
-  </si>
-  <si>
-    <t>Create collection of 5 known GPS locations on campus using Google Maps</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Code basic app that gets the current GPS location when a button is pressed, displaying it to the screen and the time from when the button was pressed to when the GPS location is acquired</t>
-  </si>
-  <si>
-    <t>Add functionality to GPS app that gets current facing direction</t>
-  </si>
-  <si>
-    <t>Test facing direction functionality</t>
-  </si>
-  <si>
-    <t>Test basic GPS locator app at known locations, comparing the results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="6">
@@ -437,9 +441,6 @@
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -534,6 +535,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -896,1366 +900,1376 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="7"/>
+    <col min="2" max="2" width="36.5703125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="6"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14" thickBot="1">
-      <c r="A1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>30</v>
+      <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="7">
+        <v>62</v>
+      </c>
+      <c r="I1" s="6">
         <f ca="1">TODAY()</f>
-        <v>40085</v>
+        <v>40089</v>
       </c>
       <c r="J1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14" thickBot="1">
+      <c r="A2" s="24" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="14" thickBot="1">
-      <c r="A2" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="22">
-        <v>0</v>
-      </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
+      <c r="B2" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="21">
+        <v>0</v>
+      </c>
+      <c r="E2" s="29"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
       <c r="H2">
         <f ca="1">IF(AND(C2&lt;$I$1,D2&lt;1),1,0)</f>
         <v>0</v>
       </c>
-      <c r="I2" s="33"/>
+      <c r="I2" s="32"/>
       <c r="J2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14" thickBot="1">
-      <c r="A3" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="A3" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4">
         <v>40101</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <f>SUMPRODUCT(D4:D8,E4:E8)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="29">
         <f>SUM(E4:E8)</f>
         <v>1</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="24"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
       <c r="H3">
         <f ca="1">IF(AND(C3&lt;$I$1,D3&lt;1),1,0)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="33"/>
+      <c r="I3" s="32"/>
       <c r="J3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="25" thickBot="1">
-      <c r="A4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="A4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
         <v>40089</v>
       </c>
-      <c r="D4" s="13">
-        <v>0</v>
-      </c>
-      <c r="E4" s="31">
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="30">
         <v>0.2</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="6"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="5"/>
       <c r="H4">
         <f ca="1">IF(AND(C4&lt;$I$1,D4&lt;1),1,0)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="33"/>
+      <c r="I4" s="32"/>
       <c r="J4">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="25" thickBot="1">
-      <c r="A5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="A5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4">
         <v>40092</v>
       </c>
-      <c r="D5" s="13">
-        <v>0</v>
-      </c>
-      <c r="E5" s="31">
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="30">
         <v>0.2</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="6"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="5"/>
       <c r="H5">
         <f t="shared" ref="H5:H50" ca="1" si="0">IF(AND(C5&lt;$I$1,D5&lt;1),1,0)</f>
         <v>0</v>
       </c>
-      <c r="I5" s="33"/>
+      <c r="I5" s="32"/>
       <c r="J5">
         <v>1.2</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14" thickBot="1">
-      <c r="A6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="A6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4">
         <v>40096</v>
       </c>
-      <c r="D6" s="13">
-        <v>0</v>
-      </c>
-      <c r="E6" s="31">
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="30">
         <v>0.25</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="6"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="5"/>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="33"/>
+      <c r="I6" s="32"/>
       <c r="J6">
         <v>1.3</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="25" thickBot="1">
-      <c r="A7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="A7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4">
         <v>40099</v>
       </c>
-      <c r="D7" s="13">
-        <v>0</v>
-      </c>
-      <c r="E7" s="31">
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+      <c r="E7" s="30">
         <v>0.1</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="6"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="5"/>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="33"/>
+      <c r="I7" s="32"/>
       <c r="J7">
         <v>1.4</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14" thickBot="1">
-      <c r="A8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="A8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4">
         <v>40101</v>
       </c>
-      <c r="D8" s="13">
-        <v>0</v>
-      </c>
-      <c r="E8" s="31">
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="30">
         <v>0.25</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="6"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="5"/>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="33"/>
+      <c r="I8" s="32"/>
       <c r="J8">
         <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14" thickBot="1">
-      <c r="A9" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="A9" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4">
         <v>40096</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <f>SUMPRODUCT(D10:D14,E10:E14)</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="30">
+        <v>1</v>
+      </c>
+      <c r="E9" s="29">
         <f>SUM(E10:E14)</f>
         <v>1</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="5"/>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="33"/>
+      <c r="I9" s="32"/>
       <c r="J9">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="25" thickBot="1">
-      <c r="A10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="A10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4">
         <v>40088</v>
       </c>
-      <c r="D10" s="13">
-        <v>0</v>
-      </c>
-      <c r="E10" s="31">
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="30">
         <v>0.1</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="6"/>
+      <c r="F10" s="8">
+        <v>40088</v>
+      </c>
+      <c r="G10" s="5"/>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="33"/>
+      <c r="I10" s="32"/>
       <c r="J10">
         <v>2.1</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14" thickBot="1">
-      <c r="A11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="A11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4">
         <v>40089</v>
       </c>
-      <c r="D11" s="13">
-        <v>0</v>
-      </c>
-      <c r="E11" s="31">
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="30">
         <v>0.3</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="8">
+        <v>40089</v>
+      </c>
+      <c r="G11" s="5"/>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="33"/>
+      <c r="I11" s="32"/>
       <c r="J11">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="25" thickBot="1">
-      <c r="A12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="A12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4">
         <v>40092</v>
       </c>
-      <c r="D12" s="13">
-        <v>0</v>
-      </c>
-      <c r="E12" s="31">
+      <c r="D12" s="12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="30">
         <v>0.15</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="6"/>
+      <c r="F12" s="8">
+        <v>40089</v>
+      </c>
+      <c r="G12" s="5"/>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="33"/>
+      <c r="I12" s="32"/>
       <c r="J12">
         <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="37" thickBot="1">
-      <c r="A13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="A13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4">
         <v>40092</v>
       </c>
-      <c r="D13" s="13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="31">
+      <c r="D13" s="12">
+        <v>1</v>
+      </c>
+      <c r="E13" s="30">
         <v>0.3</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="6"/>
+      <c r="F13" s="8">
+        <v>40089</v>
+      </c>
+      <c r="G13" s="5"/>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="33"/>
+      <c r="I13" s="32"/>
       <c r="J13">
         <v>2.4</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="25" thickBot="1">
-      <c r="A14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="A14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4">
         <v>40096</v>
       </c>
-      <c r="D14" s="13">
-        <v>0</v>
-      </c>
-      <c r="E14" s="31">
+      <c r="D14" s="12">
+        <v>1</v>
+      </c>
+      <c r="E14" s="30">
         <v>0.15</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="8">
+        <v>40089</v>
+      </c>
+      <c r="G14" s="5"/>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="33"/>
+      <c r="I14" s="32"/>
       <c r="J14">
         <v>2.5</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="14" thickBot="1">
-      <c r="A15" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="A15" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4">
         <v>40101</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="21">
         <f>SUMPRODUCT(D16:D21,E16:E21)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="30">
         <f>SUM(E16:E21)</f>
         <v>1</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="6"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="5"/>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="33"/>
+      <c r="I15" s="32"/>
       <c r="J15">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="25" thickBot="1">
-      <c r="A16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="5">
+      <c r="B16" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="4">
         <v>40088</v>
       </c>
-      <c r="D16" s="13">
-        <v>0</v>
-      </c>
-      <c r="E16" s="31">
+      <c r="D16" s="12">
+        <v>0</v>
+      </c>
+      <c r="E16" s="30">
         <v>0.1</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="6"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="5"/>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="32"/>
       <c r="J16">
         <v>3.1</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="25" thickBot="1">
-      <c r="A17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="A17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="4">
         <v>40089</v>
       </c>
-      <c r="D17" s="13">
-        <v>0</v>
-      </c>
-      <c r="E17" s="31">
+      <c r="D17" s="12">
+        <v>0</v>
+      </c>
+      <c r="E17" s="30">
         <v>0.05</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="6"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="5"/>
       <c r="H17">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="33"/>
+      <c r="I17" s="32"/>
       <c r="J17">
         <v>3.2</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="49" thickBot="1">
-      <c r="A18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="A18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4">
         <v>40095</v>
       </c>
-      <c r="D18" s="13">
-        <v>0</v>
-      </c>
-      <c r="E18" s="31">
+      <c r="D18" s="12">
+        <v>0</v>
+      </c>
+      <c r="E18" s="30">
         <v>0.4</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="6"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="5"/>
       <c r="H18">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="33"/>
+      <c r="I18" s="32"/>
       <c r="J18">
         <v>3.3</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="25" thickBot="1">
-      <c r="A19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="5">
+      <c r="A19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="4">
         <v>40096</v>
       </c>
-      <c r="D19" s="13">
-        <v>0</v>
-      </c>
-      <c r="E19" s="31">
+      <c r="D19" s="12">
+        <v>0</v>
+      </c>
+      <c r="E19" s="30">
         <v>0.1</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="6"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="5"/>
       <c r="H19">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="33"/>
+      <c r="I19" s="32"/>
       <c r="J19">
         <v>3.4</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="25" thickBot="1">
-      <c r="A20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="5">
+      <c r="A20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="4">
         <v>40099</v>
       </c>
-      <c r="D20" s="13">
-        <v>0</v>
-      </c>
-      <c r="E20" s="31">
+      <c r="D20" s="12">
+        <v>0</v>
+      </c>
+      <c r="E20" s="30">
         <v>0.25</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="6"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="5"/>
       <c r="H20">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="33"/>
+      <c r="I20" s="32"/>
       <c r="J20">
         <v>3.5</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="14" thickBot="1">
-      <c r="A21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="A21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4">
         <v>40101</v>
       </c>
-      <c r="D21" s="13">
-        <v>0</v>
-      </c>
-      <c r="E21" s="31">
+      <c r="D21" s="12">
+        <v>0</v>
+      </c>
+      <c r="E21" s="30">
         <v>0.1</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="6"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="5"/>
       <c r="H21">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="33"/>
+      <c r="I21" s="32"/>
       <c r="J21">
         <v>3.6</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14" thickBot="1">
-      <c r="A22" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="A22" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="4">
         <v>40106</v>
       </c>
-      <c r="D22" s="13">
-        <v>0</v>
-      </c>
-      <c r="E22" s="31">
+      <c r="D22" s="12">
+        <v>0</v>
+      </c>
+      <c r="E22" s="30">
         <v>1</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="6"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="5"/>
       <c r="H22">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I22" s="33"/>
+      <c r="I22" s="32"/>
       <c r="J22">
         <v>3.7</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14" thickBot="1">
-      <c r="A23" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="5">
+      <c r="A23" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="4">
         <v>40111</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="21">
         <f>SUMPRODUCT(D24:D26,E24:E26)</f>
         <v>0</v>
       </c>
-      <c r="E23" s="31">
+      <c r="E23" s="30">
         <f>SUM(E24:E26)</f>
         <v>1</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="6"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="5"/>
       <c r="H23">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23" s="33"/>
+      <c r="I23" s="32"/>
       <c r="J23">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="25" thickBot="1">
-      <c r="A24" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="A24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="4">
         <v>40106</v>
       </c>
-      <c r="D24" s="13">
-        <v>0</v>
-      </c>
-      <c r="E24" s="31">
+      <c r="D24" s="12">
+        <v>0</v>
+      </c>
+      <c r="E24" s="30">
         <v>0.4</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="6"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="5"/>
       <c r="H24">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I24" s="33"/>
+      <c r="I24" s="32"/>
       <c r="J24">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="14" thickBot="1">
-      <c r="A25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="5">
+      <c r="A25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="4">
         <v>40110</v>
       </c>
-      <c r="D25" s="13">
-        <v>0</v>
-      </c>
-      <c r="E25" s="31">
+      <c r="D25" s="12">
+        <v>0</v>
+      </c>
+      <c r="E25" s="30">
         <v>0.4</v>
       </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="6"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="5"/>
       <c r="H25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I25" s="33"/>
+      <c r="I25" s="32"/>
       <c r="J25">
         <v>4.2</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="14" thickBot="1">
-      <c r="A26" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="5">
+      <c r="A26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="4">
         <v>40111</v>
       </c>
-      <c r="D26" s="13">
-        <v>0</v>
-      </c>
-      <c r="E26" s="31">
+      <c r="D26" s="12">
+        <v>0</v>
+      </c>
+      <c r="E26" s="30">
         <v>0.2</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="6"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="5"/>
       <c r="H26">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I26" s="33"/>
+      <c r="I26" s="32"/>
       <c r="J26">
         <v>4.3</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="14" thickBot="1">
-      <c r="A27" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="5">
+      <c r="A27" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="4">
         <v>40110</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="21">
         <f>SUMPRODUCT(D28:D31,E28:E31)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="31">
+      <c r="E27" s="30">
         <f>SUM(E28:E31)</f>
         <v>1</v>
       </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="6"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="5"/>
       <c r="H27">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I27" s="33"/>
+      <c r="I27" s="32"/>
       <c r="J27">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="25" thickBot="1">
-      <c r="A28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="5">
+      <c r="A28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="4">
         <v>40107</v>
       </c>
-      <c r="D28" s="13">
-        <v>0</v>
-      </c>
-      <c r="E28" s="31">
+      <c r="D28" s="12">
+        <v>0</v>
+      </c>
+      <c r="E28" s="30">
         <v>0.3</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="6"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="5"/>
       <c r="H28">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I28" s="33"/>
+      <c r="I28" s="32"/>
       <c r="J28">
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14" thickBot="1">
-      <c r="A29" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="5">
+      <c r="A29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="4">
         <v>40109</v>
       </c>
-      <c r="D29" s="13">
-        <v>0</v>
-      </c>
-      <c r="E29" s="31">
+      <c r="D29" s="12">
+        <v>0</v>
+      </c>
+      <c r="E29" s="30">
         <v>0.2</v>
       </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="6"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="5"/>
       <c r="H29">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I29" s="33"/>
+      <c r="I29" s="32"/>
       <c r="J29">
         <v>5.2</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="14" thickBot="1">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>40110</v>
       </c>
-      <c r="D30" s="13">
-        <v>0</v>
-      </c>
-      <c r="E30" s="31">
+      <c r="D30" s="12">
+        <v>0</v>
+      </c>
+      <c r="E30" s="30">
         <v>0.3</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="6"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="5"/>
       <c r="H30">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I30" s="33"/>
+      <c r="I30" s="32"/>
       <c r="J30">
         <v>5.3</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14" thickBot="1">
-      <c r="A31" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="5">
+      <c r="A31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="4">
         <v>40110</v>
       </c>
-      <c r="D31" s="13">
-        <v>0</v>
-      </c>
-      <c r="E31" s="31">
+      <c r="D31" s="12">
+        <v>0</v>
+      </c>
+      <c r="E31" s="30">
         <v>0.2</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="6"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="5"/>
       <c r="H31">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I31" s="33"/>
+      <c r="I31" s="32"/>
       <c r="J31">
         <v>5.4</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="14" thickBot="1">
-      <c r="A32" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="5">
+      <c r="A32" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="4">
         <v>40111</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="21">
         <f>SUMPRODUCT(D33:D42,E33:E42)</f>
         <v>0</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="30">
         <f>SUM(E33:E42)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="15"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="14"/>
       <c r="H32">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I32" s="33"/>
+      <c r="I32" s="32"/>
       <c r="J32">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="14" thickBot="1">
-      <c r="A33" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="5">
+      <c r="A33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="4">
         <v>40089</v>
       </c>
-      <c r="D33" s="13">
-        <v>0</v>
-      </c>
-      <c r="E33" s="31">
+      <c r="D33" s="12">
+        <v>0</v>
+      </c>
+      <c r="E33" s="30">
         <v>0.05</v>
       </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="6"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="5"/>
       <c r="H33">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I33" s="33"/>
+      <c r="I33" s="32"/>
       <c r="J33">
         <v>6.01</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="25" thickBot="1">
-      <c r="A34" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="5">
+      <c r="A34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="4">
         <v>40095</v>
       </c>
-      <c r="D34" s="13">
-        <v>0</v>
-      </c>
-      <c r="E34" s="31">
+      <c r="D34" s="12">
+        <v>0</v>
+      </c>
+      <c r="E34" s="30">
         <v>0.15</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="6"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="5"/>
       <c r="H34">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I34" s="33"/>
+      <c r="I34" s="32"/>
       <c r="J34">
         <v>6.02</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="14" thickBot="1">
-      <c r="A35" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="5">
+      <c r="A35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="4">
         <v>40096</v>
       </c>
-      <c r="D35" s="13">
-        <v>0</v>
-      </c>
-      <c r="E35" s="31">
+      <c r="D35" s="12">
+        <v>0</v>
+      </c>
+      <c r="E35" s="30">
         <v>0.15</v>
       </c>
-      <c r="F35" s="9"/>
-      <c r="G35" s="6"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="5"/>
       <c r="H35">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I35" s="33"/>
+      <c r="I35" s="32"/>
       <c r="J35">
         <v>6.03</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="14" thickBot="1">
-      <c r="A36" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="5">
+      <c r="A36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="4">
         <v>40096</v>
       </c>
-      <c r="D36" s="13">
-        <v>0</v>
-      </c>
-      <c r="E36" s="31">
+      <c r="D36" s="12">
+        <v>0</v>
+      </c>
+      <c r="E36" s="30">
         <v>0.05</v>
       </c>
-      <c r="F36" s="9"/>
-      <c r="G36" s="35" t="s">
-        <v>16</v>
+      <c r="F36" s="8"/>
+      <c r="G36" s="34" t="s">
+        <v>47</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I36" s="33"/>
+      <c r="I36" s="32"/>
       <c r="J36">
         <v>6.04</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="14" thickBot="1">
-      <c r="A37" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="5">
+      <c r="A37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="4">
         <v>40098</v>
       </c>
-      <c r="D37" s="13">
-        <v>0</v>
-      </c>
-      <c r="E37" s="31">
+      <c r="D37" s="12">
+        <v>0</v>
+      </c>
+      <c r="E37" s="30">
         <v>0.15</v>
       </c>
-      <c r="F37" s="9"/>
-      <c r="G37" s="6"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="5"/>
       <c r="H37">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="33"/>
+      <c r="I37" s="32"/>
       <c r="J37">
         <v>6.05</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="14" thickBot="1">
-      <c r="A38" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="5">
+      <c r="A38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="4">
         <v>40099</v>
       </c>
-      <c r="D38" s="13">
-        <v>0</v>
-      </c>
-      <c r="E38" s="31">
+      <c r="D38" s="12">
+        <v>0</v>
+      </c>
+      <c r="E38" s="30">
         <v>0.1</v>
       </c>
-      <c r="F38" s="9"/>
-      <c r="G38" s="6"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="5"/>
       <c r="H38">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I38" s="33"/>
+      <c r="I38" s="32"/>
       <c r="J38">
         <v>6.06</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="25" thickBot="1">
-      <c r="A39" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="5">
+      <c r="A39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="4">
         <v>40101</v>
       </c>
-      <c r="D39" s="13">
-        <v>0</v>
-      </c>
-      <c r="E39" s="31">
+      <c r="D39" s="12">
+        <v>0</v>
+      </c>
+      <c r="E39" s="30">
         <v>0.1</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="6"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="5"/>
       <c r="H39">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I39" s="33"/>
+      <c r="I39" s="32"/>
       <c r="J39">
         <v>6.07</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="25" thickBot="1">
-      <c r="A40" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="5">
+      <c r="A40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="4">
         <v>40106</v>
       </c>
-      <c r="D40" s="13">
-        <v>0</v>
-      </c>
-      <c r="E40" s="31">
+      <c r="D40" s="12">
+        <v>0</v>
+      </c>
+      <c r="E40" s="30">
         <v>0.05</v>
       </c>
-      <c r="F40" s="9"/>
-      <c r="G40" s="6"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="5"/>
       <c r="H40">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I40" s="33"/>
+      <c r="I40" s="32"/>
       <c r="J40">
         <v>6.08</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="25" thickBot="1">
-      <c r="A41" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="5">
+      <c r="A41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="4">
         <v>40110</v>
       </c>
-      <c r="D41" s="13">
-        <v>0</v>
-      </c>
-      <c r="E41" s="31">
+      <c r="D41" s="12">
+        <v>0</v>
+      </c>
+      <c r="E41" s="30">
         <v>0.1</v>
       </c>
-      <c r="F41" s="9"/>
-      <c r="G41" s="6"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="5"/>
       <c r="H41">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I41" s="33"/>
+      <c r="I41" s="32"/>
       <c r="J41">
         <v>6.09</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="14" thickBot="1">
-      <c r="A42" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="5">
+      <c r="A42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="4">
         <v>40111</v>
       </c>
-      <c r="D42" s="13">
-        <v>0</v>
-      </c>
-      <c r="E42" s="31">
+      <c r="D42" s="12">
+        <v>0</v>
+      </c>
+      <c r="E42" s="30">
         <v>0.1</v>
       </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="6"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="5"/>
       <c r="H42">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I42" s="33"/>
+      <c r="I42" s="32"/>
       <c r="J42">
         <v>6.1</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="14" thickBot="1">
-      <c r="A43" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" s="5">
+      <c r="A43" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="4">
         <v>40112</v>
       </c>
-      <c r="D43" s="22">
+      <c r="D43" s="21">
         <f>SUMPRODUCT(D44:D46,E44:E46)</f>
         <v>0</v>
       </c>
-      <c r="E43" s="31">
+      <c r="E43" s="30">
         <f>SUM(E44:E46)</f>
         <v>1</v>
       </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="6"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="5"/>
       <c r="H43">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I43" s="33"/>
+      <c r="I43" s="32"/>
       <c r="J43">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="25" thickBot="1">
-      <c r="A44" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="5">
+      <c r="A44" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="4">
         <v>40109</v>
       </c>
-      <c r="D44" s="13">
-        <v>0</v>
-      </c>
-      <c r="E44" s="31">
+      <c r="D44" s="12">
+        <v>0</v>
+      </c>
+      <c r="E44" s="30">
         <v>0.2</v>
       </c>
-      <c r="F44" s="9"/>
-      <c r="G44" s="6"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="5"/>
       <c r="H44">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I44" s="33"/>
+      <c r="I44" s="32"/>
       <c r="J44">
         <v>7.1</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="37" thickBot="1">
-      <c r="A45" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C45" s="5">
+      <c r="A45" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="4">
         <v>40111</v>
       </c>
-      <c r="D45" s="13">
-        <v>0</v>
-      </c>
-      <c r="E45" s="31">
+      <c r="D45" s="12">
+        <v>0</v>
+      </c>
+      <c r="E45" s="30">
         <v>0.5</v>
       </c>
-      <c r="F45" s="9"/>
-      <c r="G45" s="6"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="5"/>
       <c r="H45">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I45" s="33"/>
+      <c r="I45" s="32"/>
       <c r="J45">
         <v>7.2</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="25" thickBot="1">
-      <c r="A46" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="5">
+      <c r="A46" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="4">
         <v>40112</v>
       </c>
-      <c r="D46" s="13">
-        <v>0</v>
-      </c>
-      <c r="E46" s="31">
+      <c r="D46" s="12">
+        <v>0</v>
+      </c>
+      <c r="E46" s="30">
         <v>0.3</v>
       </c>
-      <c r="F46" s="9"/>
-      <c r="G46" s="6"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="5"/>
       <c r="H46">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I46" s="33"/>
+      <c r="I46" s="32"/>
       <c r="J46">
         <v>7.3</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="14" thickBot="1">
-      <c r="A47" s="4"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="6"/>
-      <c r="I47" s="33"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="5"/>
+      <c r="I47" s="32"/>
     </row>
     <row r="48" spans="1:10" ht="14" thickBot="1">
-      <c r="A48" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" s="5">
+      <c r="A48" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="4">
         <v>40115</v>
       </c>
-      <c r="D48" s="13">
-        <v>0</v>
-      </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="6"/>
+      <c r="D48" s="12">
+        <v>0</v>
+      </c>
+      <c r="E48" s="30"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="5"/>
       <c r="H48">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I48" s="33"/>
+      <c r="I48" s="32"/>
     </row>
     <row r="49" spans="1:9" ht="14" thickBot="1">
-      <c r="A49" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="5">
+      <c r="A49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="4">
         <v>40115</v>
       </c>
-      <c r="D49" s="13">
-        <v>0</v>
-      </c>
-      <c r="E49" s="31"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="6"/>
+      <c r="D49" s="12">
+        <v>0</v>
+      </c>
+      <c r="E49" s="30"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="5"/>
       <c r="H49">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I49" s="33"/>
+      <c r="I49" s="32"/>
     </row>
     <row r="50" spans="1:9" ht="14" thickBot="1">
-      <c r="A50" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="5">
+      <c r="A50" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="4">
         <v>40115</v>
       </c>
-      <c r="D50" s="13">
-        <v>0</v>
-      </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="6"/>
+      <c r="D50" s="12">
+        <v>0</v>
+      </c>
+      <c r="E50" s="30"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="5"/>
       <c r="H50">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I50" s="33"/>
+      <c r="I50" s="32"/>
     </row>
     <row r="51" spans="1:9" ht="14" thickBot="1">
-      <c r="A51" s="4"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="5"/>
-      <c r="I51" s="33"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="4"/>
+      <c r="I51" s="32"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2297,25 +2311,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
+      <c r="A1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" thickBot="1">
-      <c r="A2" s="17" t="s">
-        <v>48</v>
+      <c r="A2" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -2323,127 +2337,127 @@
       <c r="E2" s="37"/>
     </row>
     <row r="3" spans="1:5" ht="14" thickBot="1">
-      <c r="A3" s="17">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="17">
         <v>0.2</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <v>10</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="17">
         <v>1</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <f>B3*D3/C3</f>
         <v>0.02</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14" thickBot="1">
-      <c r="A4" s="17">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <v>0.2</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>12</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>0.9</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f t="shared" ref="E4:E9" si="0">B4*D4/C4</f>
         <v>1.5000000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14" thickBot="1">
-      <c r="A5" s="17">
+      <c r="A5" s="16">
         <v>3</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>0.15</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>7</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>0.5</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <f t="shared" si="0"/>
         <v>1.0714285714285714E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14" thickBot="1">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>4</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>0.1</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>10</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>0.4</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <f t="shared" si="0"/>
         <v>4.000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14" thickBot="1">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>5</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <v>0.1</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <v>5</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>0.8</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <f t="shared" si="0"/>
         <v>1.6000000000000004E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14" thickBot="1">
-      <c r="A8" s="17">
+      <c r="A8" s="16">
         <v>6</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="17">
         <v>0.1</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <v>15</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>0.6</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <f t="shared" si="0"/>
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14" thickBot="1">
-      <c r="A9" s="17">
+      <c r="A9" s="16">
         <v>7</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="17">
         <v>0.15</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>6</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>0.6</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>

</xml_diff>

<commit_message>
Finish integration of basic GPS code, begin code for movement
</commit_message>
<xml_diff>
--- a/Documentation/Project2TasksSpreadsheet.xlsx
+++ b/Documentation/Project2TasksSpreadsheet.xlsx
@@ -22,6 +22,127 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="74">
   <si>
+    <t>Modify robot frame to attempt to fix issue with robot veering left</t>
+  </si>
+  <si>
+    <t>If necessary tune motors to get robot to move straight</t>
+  </si>
+  <si>
+    <t>Test moving straight for 20m inside</t>
+  </si>
+  <si>
+    <t>Test moving straight for 20m outside</t>
+  </si>
+  <si>
+    <t>Robot uses sensors (3 sensors)</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Robot moves in a straight line</t>
+  </si>
+  <si>
+    <t>Read API for Ultrasonic sensor (CSonar, CSonarController)</t>
+  </si>
+  <si>
+    <t>Implement group of sonar sensors (forward, backward, down facing both front and back) using interrupts</t>
+  </si>
+  <si>
+    <t>Test Sonar implmentation</t>
+  </si>
+  <si>
+    <t>Read examples on how to use the optical encoders</t>
+  </si>
+  <si>
+    <t>https://code.google.com/p/terkos/source/browse/trunk/src/examples/linux/SonarRover/encoder.h?r=1216</t>
+  </si>
+  <si>
+    <t>Code reading data from the optical encoders</t>
+  </si>
+  <si>
+    <t>Test reading data from the optical encoders</t>
+  </si>
+  <si>
+    <t>Determine third sensor to use with the Vex and how this sensor can help us</t>
+  </si>
+  <si>
+    <t>Test reading data from the sensor and using it in some way</t>
+  </si>
+  <si>
+    <t>Determine use for data from optical encoders caode and test using this data in some way related to this</t>
+  </si>
+  <si>
+    <t>Code reading data from this sensor and using it for something</t>
+  </si>
+  <si>
+    <t>Cliff test</t>
+  </si>
+  <si>
+    <t>Determine highest possible drop that the Vex can navigate safely</t>
+  </si>
+  <si>
+    <t>Use Sonar implementation to use downward facing sensors to check if the robot is about to go over a drop greater than or equal to this distance</t>
+  </si>
+  <si>
+    <t>Test cliff sensors</t>
+  </si>
+  <si>
+    <t>Alex
+(Sei Jung)</t>
+  </si>
+  <si>
+    <t>%Complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date Complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Today:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Who</t>
+  </si>
+  <si>
+    <t>What</t>
+  </si>
+  <si>
+    <t>When</t>
+  </si>
+  <si>
+    <t>Sei Jung</t>
+  </si>
+  <si>
+    <t>Jerrell</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Ensure all devices are secured in storage</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>Merge Project code to final projects for submittal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Report</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Jacob</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -132,138 +253,13 @@
   </si>
   <si>
     <t>Test moving to a GPS Coordinate</t>
-  </si>
-  <si>
-    <t>Modify robot frame to attempt to fix issue with robot veering left</t>
-  </si>
-  <si>
-    <t>If necessary tune motors to get robot to move straight</t>
-  </si>
-  <si>
-    <t>Test moving straight for 20m inside</t>
-  </si>
-  <si>
-    <t>Test moving straight for 20m outside</t>
-  </si>
-  <si>
-    <t>Robot uses sensors (3 sensors)</t>
-  </si>
-  <si>
-    <t>Requirement</t>
-  </si>
-  <si>
-    <t>Robot moves in a straight line</t>
-  </si>
-  <si>
-    <t>Read API for Ultrasonic sensor (CSonar, CSonarController)</t>
-  </si>
-  <si>
-    <t>Implement group of sonar sensors (forward, backward, down facing both front and back) using interrupts</t>
-  </si>
-  <si>
-    <t>Test Sonar implmentation</t>
-  </si>
-  <si>
-    <t>Read examples on how to use the optical encoders</t>
-  </si>
-  <si>
-    <t>https://code.google.com/p/terkos/source/browse/trunk/src/examples/linux/SonarRover/encoder.h?r=1216</t>
-  </si>
-  <si>
-    <t>Code reading data from the optical encoders</t>
-  </si>
-  <si>
-    <t>Test reading data from the optical encoders</t>
-  </si>
-  <si>
-    <t>Determine third sensor to use with the Vex and how this sensor can help us</t>
-  </si>
-  <si>
-    <t>Test reading data from the sensor and using it in some way</t>
-  </si>
-  <si>
-    <t>Determine use for data from optical encoders caode and test using this data in some way related to this</t>
-  </si>
-  <si>
-    <t>Code reading data from this sensor and using it for something</t>
-  </si>
-  <si>
-    <t>Cliff test</t>
-  </si>
-  <si>
-    <t>Determine highest possible drop that the Vex can navigate safely</t>
-  </si>
-  <si>
-    <t>Use Sonar implementation to use downward facing sensors to check if the robot is about to go over a drop greater than or equal to this distance</t>
-  </si>
-  <si>
-    <t>Test cliff sensors</t>
-  </si>
-  <si>
-    <t>Alex
-(Sei Jung)</t>
-  </si>
-  <si>
-    <t>%Complete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date Complete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Notes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Today:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Who</t>
-  </si>
-  <si>
-    <t>What</t>
-  </si>
-  <si>
-    <t>When</t>
-  </si>
-  <si>
-    <t>Sei Jung</t>
-  </si>
-  <si>
-    <t>Jerrell</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Jacob</t>
-  </si>
-  <si>
-    <t>Ensure all devices are secured in storage</t>
-  </si>
-  <si>
-    <t>ongoing</t>
-  </si>
-  <si>
-    <t>Merge Project code to final projects for submittal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Report</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="6">
@@ -899,8 +895,8 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
@@ -915,46 +911,46 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>26</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" t="s">
-        <v>62</v>
       </c>
       <c r="I1" s="6">
         <f ca="1">TODAY()</f>
-        <v>40089</v>
+        <v>40107</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14" thickBot="1">
       <c r="A2" s="24" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="D2" s="21">
         <v>0</v>
@@ -973,10 +969,10 @@
     </row>
     <row r="3" spans="1:10" ht="14" thickBot="1">
       <c r="A3" s="27" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C3" s="4">
         <v>40101</v>
@@ -993,7 +989,7 @@
       <c r="G3" s="23"/>
       <c r="H3">
         <f ca="1">IF(AND(C3&lt;$I$1,D3&lt;1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="32"/>
       <c r="J3">
@@ -1002,10 +998,10 @@
     </row>
     <row r="4" spans="1:10" ht="25" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="C4" s="4">
         <v>40089</v>
@@ -1020,7 +1016,7 @@
       <c r="G4" s="5"/>
       <c r="H4">
         <f ca="1">IF(AND(C4&lt;$I$1,D4&lt;1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="32"/>
       <c r="J4">
@@ -1029,10 +1025,10 @@
     </row>
     <row r="5" spans="1:10" ht="25" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C5" s="4">
         <v>40092</v>
@@ -1047,7 +1043,7 @@
       <c r="G5" s="5"/>
       <c r="H5">
         <f t="shared" ref="H5:H50" ca="1" si="0">IF(AND(C5&lt;$I$1,D5&lt;1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="32"/>
       <c r="J5">
@@ -1056,10 +1052,10 @@
     </row>
     <row r="6" spans="1:10" ht="14" thickBot="1">
       <c r="A6" s="3" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C6" s="4">
         <v>40096</v>
@@ -1074,7 +1070,7 @@
       <c r="G6" s="5"/>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="32"/>
       <c r="J6">
@@ -1083,10 +1079,10 @@
     </row>
     <row r="7" spans="1:10" ht="25" thickBot="1">
       <c r="A7" s="3" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C7" s="4">
         <v>40099</v>
@@ -1101,7 +1097,7 @@
       <c r="G7" s="5"/>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="32"/>
       <c r="J7">
@@ -1110,10 +1106,10 @@
     </row>
     <row r="8" spans="1:10" ht="14" thickBot="1">
       <c r="A8" s="3" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C8" s="4">
         <v>40101</v>
@@ -1128,7 +1124,7 @@
       <c r="G8" s="5"/>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="32"/>
       <c r="J8">
@@ -1137,10 +1133,10 @@
     </row>
     <row r="9" spans="1:10" ht="14" thickBot="1">
       <c r="A9" s="27" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="C9" s="4">
         <v>40096</v>
@@ -1166,10 +1162,10 @@
     </row>
     <row r="10" spans="1:10" ht="25" thickBot="1">
       <c r="A10" s="3" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="C10" s="4">
         <v>40088</v>
@@ -1195,10 +1191,10 @@
     </row>
     <row r="11" spans="1:10" ht="14" thickBot="1">
       <c r="A11" s="3" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="C11" s="4">
         <v>40089</v>
@@ -1224,10 +1220,10 @@
     </row>
     <row r="12" spans="1:10" ht="25" thickBot="1">
       <c r="A12" s="3" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="C12" s="4">
         <v>40092</v>
@@ -1253,10 +1249,10 @@
     </row>
     <row r="13" spans="1:10" ht="37" thickBot="1">
       <c r="A13" s="3" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C13" s="4">
         <v>40092</v>
@@ -1282,10 +1278,10 @@
     </row>
     <row r="14" spans="1:10" ht="25" thickBot="1">
       <c r="A14" s="3" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="C14" s="4">
         <v>40096</v>
@@ -1311,10 +1307,10 @@
     </row>
     <row r="15" spans="1:10" ht="14" thickBot="1">
       <c r="A15" s="27" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="C15" s="4">
         <v>40101</v>
@@ -1331,7 +1327,7 @@
       <c r="G15" s="5"/>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15">
@@ -1340,10 +1336,10 @@
     </row>
     <row r="16" spans="1:10" ht="25" thickBot="1">
       <c r="A16" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C16" s="4">
         <v>40088</v>
@@ -1367,10 +1363,10 @@
     </row>
     <row r="17" spans="1:10" ht="25" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C17" s="4">
         <v>40089</v>
@@ -1385,7 +1381,7 @@
       <c r="G17" s="5"/>
       <c r="H17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17">
@@ -1394,10 +1390,10 @@
     </row>
     <row r="18" spans="1:10" ht="49" thickBot="1">
       <c r="A18" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="C18" s="4">
         <v>40095</v>
@@ -1412,7 +1408,7 @@
       <c r="G18" s="5"/>
       <c r="H18">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18">
@@ -1421,10 +1417,10 @@
     </row>
     <row r="19" spans="1:10" ht="25" thickBot="1">
       <c r="A19" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="C19" s="4">
         <v>40096</v>
@@ -1439,7 +1435,7 @@
       <c r="G19" s="5"/>
       <c r="H19">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19">
@@ -1448,10 +1444,10 @@
     </row>
     <row r="20" spans="1:10" ht="25" thickBot="1">
       <c r="A20" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="C20" s="4">
         <v>40099</v>
@@ -1466,7 +1462,7 @@
       <c r="G20" s="5"/>
       <c r="H20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20">
@@ -1475,10 +1471,10 @@
     </row>
     <row r="21" spans="1:10" ht="14" thickBot="1">
       <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>29</v>
       </c>
       <c r="C21" s="4">
         <v>40101</v>
@@ -1493,7 +1489,7 @@
       <c r="G21" s="5"/>
       <c r="H21">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21">
@@ -1502,21 +1498,23 @@
     </row>
     <row r="22" spans="1:10" ht="14" thickBot="1">
       <c r="A22" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>31</v>
       </c>
       <c r="C22" s="4">
         <v>40106</v>
       </c>
       <c r="D22" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="30">
         <v>1</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="8">
+        <v>40107</v>
+      </c>
       <c r="G22" s="5"/>
       <c r="H22">
         <f t="shared" ca="1" si="0"/>
@@ -1529,17 +1527,17 @@
     </row>
     <row r="23" spans="1:10" ht="14" thickBot="1">
       <c r="A23" s="27" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="C23" s="4">
         <v>40111</v>
       </c>
       <c r="D23" s="21">
         <f>SUMPRODUCT(D24:D26,E24:E26)</f>
-        <v>0</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="E23" s="30">
         <f>SUM(E24:E26)</f>
@@ -1558,10 +1556,10 @@
     </row>
     <row r="24" spans="1:10" ht="25" thickBot="1">
       <c r="A24" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="C24" s="4">
         <v>40106</v>
@@ -1576,7 +1574,7 @@
       <c r="G24" s="5"/>
       <c r="H24">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="32"/>
       <c r="J24">
@@ -1585,16 +1583,16 @@
     </row>
     <row r="25" spans="1:10" ht="14" thickBot="1">
       <c r="A25" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="C25" s="4">
         <v>40110</v>
       </c>
       <c r="D25" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E25" s="30">
         <v>0.4</v>
@@ -1612,10 +1610,10 @@
     </row>
     <row r="26" spans="1:10" ht="14" thickBot="1">
       <c r="A26" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="C26" s="4">
         <v>40111</v>
@@ -1639,10 +1637,10 @@
     </row>
     <row r="27" spans="1:10" ht="14" thickBot="1">
       <c r="A27" s="27" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C27" s="4">
         <v>40110</v>
@@ -1668,10 +1666,10 @@
     </row>
     <row r="28" spans="1:10" ht="25" thickBot="1">
       <c r="A28" s="3" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C28" s="4">
         <v>40107</v>
@@ -1695,10 +1693,10 @@
     </row>
     <row r="29" spans="1:10" ht="14" thickBot="1">
       <c r="A29" s="3" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C29" s="4">
         <v>40109</v>
@@ -1722,10 +1720,10 @@
     </row>
     <row r="30" spans="1:10" ht="14" thickBot="1">
       <c r="A30" s="3" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="C30" s="4">
         <v>40110</v>
@@ -1749,10 +1747,10 @@
     </row>
     <row r="31" spans="1:10" ht="14" thickBot="1">
       <c r="A31" s="3" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="C31" s="4">
         <v>40110</v>
@@ -1776,10 +1774,10 @@
     </row>
     <row r="32" spans="1:10" ht="14" thickBot="1">
       <c r="A32" s="27" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C32" s="4">
         <v>40111</v>
@@ -1805,10 +1803,10 @@
     </row>
     <row r="33" spans="1:10" ht="14" thickBot="1">
       <c r="A33" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="C33" s="4">
         <v>40089</v>
@@ -1823,7 +1821,7 @@
       <c r="G33" s="5"/>
       <c r="H33">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="32"/>
       <c r="J33">
@@ -1832,10 +1830,10 @@
     </row>
     <row r="34" spans="1:10" ht="25" thickBot="1">
       <c r="A34" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="C34" s="4">
         <v>40095</v>
@@ -1850,7 +1848,7 @@
       <c r="G34" s="5"/>
       <c r="H34">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="32"/>
       <c r="J34">
@@ -1859,10 +1857,10 @@
     </row>
     <row r="35" spans="1:10" ht="14" thickBot="1">
       <c r="A35" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C35" s="4">
         <v>40096</v>
@@ -1877,7 +1875,7 @@
       <c r="G35" s="5"/>
       <c r="H35">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="32"/>
       <c r="J35">
@@ -1886,10 +1884,10 @@
     </row>
     <row r="36" spans="1:10" ht="14" thickBot="1">
       <c r="A36" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C36" s="4">
         <v>40096</v>
@@ -1902,11 +1900,11 @@
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="34" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="32"/>
       <c r="J36">
@@ -1915,10 +1913,10 @@
     </row>
     <row r="37" spans="1:10" ht="14" thickBot="1">
       <c r="A37" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="C37" s="4">
         <v>40098</v>
@@ -1933,7 +1931,7 @@
       <c r="G37" s="5"/>
       <c r="H37">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="32"/>
       <c r="J37">
@@ -1942,10 +1940,10 @@
     </row>
     <row r="38" spans="1:10" ht="14" thickBot="1">
       <c r="A38" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="C38" s="4">
         <v>40099</v>
@@ -1960,7 +1958,7 @@
       <c r="G38" s="5"/>
       <c r="H38">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="32"/>
       <c r="J38">
@@ -1969,10 +1967,10 @@
     </row>
     <row r="39" spans="1:10" ht="25" thickBot="1">
       <c r="A39" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="C39" s="4">
         <v>40101</v>
@@ -1987,7 +1985,7 @@
       <c r="G39" s="5"/>
       <c r="H39">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="32"/>
       <c r="J39">
@@ -1996,10 +1994,10 @@
     </row>
     <row r="40" spans="1:10" ht="25" thickBot="1">
       <c r="A40" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C40" s="4">
         <v>40106</v>
@@ -2014,7 +2012,7 @@
       <c r="G40" s="5"/>
       <c r="H40">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="32"/>
       <c r="J40">
@@ -2023,10 +2021,10 @@
     </row>
     <row r="41" spans="1:10" ht="25" thickBot="1">
       <c r="A41" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="C41" s="4">
         <v>40110</v>
@@ -2050,10 +2048,10 @@
     </row>
     <row r="42" spans="1:10" ht="14" thickBot="1">
       <c r="A42" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="C42" s="4">
         <v>40111</v>
@@ -2077,10 +2075,10 @@
     </row>
     <row r="43" spans="1:10" ht="14" thickBot="1">
       <c r="A43" s="27" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C43" s="4">
         <v>40112</v>
@@ -2106,10 +2104,10 @@
     </row>
     <row r="44" spans="1:10" ht="25" thickBot="1">
       <c r="A44" s="35" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C44" s="4">
         <v>40109</v>
@@ -2133,10 +2131,10 @@
     </row>
     <row r="45" spans="1:10" ht="37" thickBot="1">
       <c r="A45" s="35" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="C45" s="4">
         <v>40111</v>
@@ -2160,10 +2158,10 @@
     </row>
     <row r="46" spans="1:10" ht="25" thickBot="1">
       <c r="A46" s="35" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="C46" s="4">
         <v>40112</v>
@@ -2197,10 +2195,10 @@
     </row>
     <row r="48" spans="1:10" ht="14" thickBot="1">
       <c r="A48" s="3" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="C48" s="4">
         <v>40115</v>
@@ -2219,10 +2217,10 @@
     </row>
     <row r="49" spans="1:9" ht="14" thickBot="1">
       <c r="A49" s="3" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="C49" s="4">
         <v>40115</v>
@@ -2241,10 +2239,10 @@
     </row>
     <row r="50" spans="1:9" ht="14" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C50" s="4">
         <v>40115</v>
@@ -2272,6 +2270,7 @@
       <c r="I51" s="32"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C3:C51">
     <cfRule type="expression" dxfId="1" priority="0" stopIfTrue="1">
@@ -2312,24 +2311,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="15" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" thickBot="1">
       <c r="A2" s="16" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -2463,6 +2462,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>

</xml_diff>